<commit_message>
K_s values update and vertical composite design update
</commit_message>
<xml_diff>
--- a/PreliminaryAirframe/Composite/Composite_vertical_tailplane_sizing.xlsx
+++ b/PreliminaryAirframe/Composite/Composite_vertical_tailplane_sizing.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ca90458c880e139/Documents/GitHub/AVD/PreliminaryAirframe/Composite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1155" documentId="8_{F426B969-63F3-4CD9-9347-CB9329FBF99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF5DBCAB-861D-4279-9556-8E30B41B5408}"/>
+  <xr:revisionPtr revIDLastSave="1682" documentId="8_{F426B969-63F3-4CD9-9347-CB9329FBF99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{597C73AA-F51C-4C61-A072-906B7AED6B23}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E7E02545-2DF6-46D5-87DA-A9BD6A8E819A}"/>
+    <workbookView xWindow="-11550" yWindow="3623" windowWidth="19200" windowHeight="8422" firstSheet="1" activeTab="4" xr2:uid="{E7E02545-2DF6-46D5-87DA-A9BD6A8E819A}"/>
   </bookViews>
   <sheets>
     <sheet name="1. 0 ribs" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Panel V2" sheetId="3" r:id="rId3"/>
+    <sheet name="Panel Design V2" sheetId="4" r:id="rId4"/>
+    <sheet name="D-CELL V2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="198">
   <si>
     <t>Composite Wingbox sizing</t>
   </si>
@@ -441,6 +444,195 @@
   </si>
   <si>
     <t>l3</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>denominator 1 (max)</t>
+  </si>
+  <si>
+    <t>denominator 2 (min)</t>
+  </si>
+  <si>
+    <t>Nx,cl, cr (max) [N]</t>
+  </si>
+  <si>
+    <t>Ny,cl,cr (max) [N]</t>
+  </si>
+  <si>
+    <t>Nx,cl,cr (min) [N]</t>
+  </si>
+  <si>
+    <t>Ny,cl,cr (min) [N]</t>
+  </si>
+  <si>
+    <t>XAS/913 1</t>
+  </si>
+  <si>
+    <t>N_x</t>
+  </si>
+  <si>
+    <t>N_y</t>
+  </si>
+  <si>
+    <t>b min [m]</t>
+  </si>
+  <si>
+    <t>b max [m]</t>
+  </si>
+  <si>
+    <t>a [m]</t>
+  </si>
+  <si>
+    <t>b max/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b min/a </t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T1 max</t>
+  </si>
+  <si>
+    <t>NUMERATOR max</t>
+  </si>
+  <si>
+    <t>T2 max</t>
+  </si>
+  <si>
+    <t>T1 min</t>
+  </si>
+  <si>
+    <t>T2 min</t>
+  </si>
+  <si>
+    <t>NUMERATOR min</t>
+  </si>
+  <si>
+    <t>t1 [m]</t>
+  </si>
+  <si>
+    <t>c max</t>
+  </si>
+  <si>
+    <t>c min</t>
+  </si>
+  <si>
+    <t>r1 [m] min</t>
+  </si>
+  <si>
+    <t>r1 [m] max</t>
+  </si>
+  <si>
+    <t>a/(b max)</t>
+  </si>
+  <si>
+    <t>a/(b min)</t>
+  </si>
+  <si>
+    <t>a greater than b</t>
+  </si>
+  <si>
+    <t>x (b min)</t>
+  </si>
+  <si>
+    <t>x (b max)</t>
+  </si>
+  <si>
+    <t>E panel</t>
+  </si>
+  <si>
+    <t>tau_cr (b min)</t>
+  </si>
+  <si>
+    <t>tau_cr (b max)</t>
+  </si>
+  <si>
+    <t>E_xx</t>
+  </si>
+  <si>
+    <t>E_yy</t>
+  </si>
+  <si>
+    <t>G_xy</t>
+  </si>
+  <si>
+    <t>v_xy</t>
+  </si>
+  <si>
+    <t>v_yx</t>
+  </si>
+  <si>
+    <t>N_xx</t>
+  </si>
+  <si>
+    <t>N_yy</t>
+  </si>
+  <si>
+    <t>N_xy</t>
+  </si>
+  <si>
+    <t>vf</t>
+  </si>
+  <si>
+    <t>vm</t>
+  </si>
+  <si>
+    <t>E max</t>
+  </si>
+  <si>
+    <t>E min</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>sigma_11 t</t>
+  </si>
+  <si>
+    <t>sigma_11 c</t>
+  </si>
+  <si>
+    <t>Material Properties -XAS/914</t>
+  </si>
+  <si>
+    <t>sigma_22 t</t>
+  </si>
+  <si>
+    <t>sigma_22 c</t>
+  </si>
+  <si>
+    <t>sigma_12</t>
+  </si>
+  <si>
+    <t>K_s (min)</t>
+  </si>
+  <si>
+    <t>K_s (max)</t>
+  </si>
+  <si>
+    <t>M_max</t>
+  </si>
+  <si>
+    <t>Nm</t>
+  </si>
+  <si>
+    <t>A 914</t>
+  </si>
+  <si>
+    <t>3.54 Mpa</t>
+  </si>
+  <si>
+    <t>2.91 Mpa</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD7C898-DEA3-436A-978C-3D1D23C43CFE}">
   <dimension ref="A1:AL76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="M7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1477,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="18">
-        <f t="shared" ref="S10:S19" si="2">2*ROUNDUP(0.1*P10, 0)</f>
+        <f t="shared" ref="S10:S11" si="2">2*ROUNDUP(0.1*P10, 0)</f>
         <v>2</v>
       </c>
       <c r="T10" s="19">
@@ -1492,14 +1684,14 @@
         <v>2</v>
       </c>
       <c r="W10" s="21">
-        <f t="shared" ref="W10:W12" si="4">$B$5*V10</f>
+        <f t="shared" ref="W10:W11" si="4">$B$5*V10</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="X10" s="22">
         <v>0</v>
       </c>
       <c r="Y10" s="15">
-        <f t="shared" ref="Y10:Y19" si="5">2*ROUNDUP(0.1*AE10, 0)</f>
+        <f t="shared" ref="Y10:Y11" si="5">2*ROUNDUP(0.1*AE10, 0)</f>
         <v>2</v>
       </c>
       <c r="Z10" s="14">
@@ -1522,7 +1714,7 @@
         <v>5.8602170000000002E-2</v>
       </c>
       <c r="AE10" s="15">
-        <f t="shared" ref="AE10:AE19" si="9">2*ROUNDUP(AD10,0)</f>
+        <f t="shared" ref="AE10:AE11" si="9">2*ROUNDUP(AD10,0)</f>
         <v>2</v>
       </c>
       <c r="AF10" s="21">
@@ -1545,7 +1737,7 @@
         <v>-6.8199999999999997E-2</v>
       </c>
       <c r="E11" s="59">
-        <f t="shared" ref="E10:E11" si="11">2*L11*C11</f>
+        <f t="shared" ref="E11" si="11">2*L11*C11</f>
         <v>0.79440120262799985</v>
       </c>
       <c r="F11">
@@ -1602,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="18">
-        <f t="shared" ref="V11:V19" si="12">2*ROUNDUP(0.1*P11, 0)</f>
+        <f t="shared" ref="V11" si="12">2*ROUNDUP(0.1*P11, 0)</f>
         <v>2</v>
       </c>
       <c r="W11" s="21">
@@ -1624,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="18">
-        <f t="shared" ref="AB11:AB19" si="13">2*ROUNDUP(0.1*AE11, 0)</f>
+        <f t="shared" ref="AB11" si="13">2*ROUNDUP(0.1*AE11, 0)</f>
         <v>2</v>
       </c>
       <c r="AC11" s="19">
@@ -3120,95 +3312,95 @@
         <v>48</v>
       </c>
       <c r="P46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(P41*P42)+P43+2*P44)</f>
+        <f t="shared" ref="P46:AL46" si="15">((2*PI()^2)/($G$15^2))*(SQRT(P41*P42)+P43+2*P44)</f>
         <v>97.724461779731527</v>
       </c>
       <c r="Q46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(Q41*Q42)+Q43+2*Q44)</f>
+        <f t="shared" si="15"/>
         <v>236.43156476384573</v>
       </c>
       <c r="R46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(R41*R42)+R43+2*R44)</f>
+        <f t="shared" si="15"/>
         <v>401.424568303466</v>
       </c>
       <c r="S46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(S41*S42)+S43+2*S44)</f>
+        <f t="shared" si="15"/>
         <v>389.6577755404395</v>
       </c>
       <c r="T46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(T41*T42)+T43+2*T44)</f>
+        <f t="shared" si="15"/>
         <v>603.74204344225973</v>
       </c>
       <c r="U46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(U41*U42)+U43+2*U44)</f>
+        <f t="shared" si="15"/>
         <v>975.95846372331107</v>
       </c>
       <c r="V46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(V41*V42)+V43+2*V44)</f>
+        <f t="shared" si="15"/>
         <v>987.22681153796339</v>
       </c>
       <c r="W46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(W41*W42)+W43+2*W44)</f>
+        <f t="shared" si="15"/>
         <v>1258.0919886872862</v>
       </c>
       <c r="X46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(X41*X42)+X43+2*X44)</f>
+        <f t="shared" si="15"/>
         <v>1641.5478449889049</v>
       </c>
       <c r="Y46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(Y41*Y42)+Y43+2*Y44)</f>
+        <f t="shared" si="15"/>
         <v>2369.2821056562352</v>
       </c>
       <c r="Z46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(Z41*Z42)+Z43+2*Z44)</f>
+        <f t="shared" si="15"/>
         <v>3242.0767354394634</v>
       </c>
       <c r="AA46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AA41*AA42)+AA43+2*AA44)</f>
+        <f t="shared" si="15"/>
         <v>3842.9930008097676</v>
       </c>
       <c r="AB46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AB41*AB42)+AB43+2*AB44)</f>
+        <f t="shared" si="15"/>
         <v>4606.4895796498276</v>
       </c>
       <c r="AC46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AC41*AC42)+AC43+2*AC44)</f>
+        <f t="shared" si="15"/>
         <v>5993.5180016565046</v>
       </c>
       <c r="AD46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AD41*AD42)+AD43+2*AD44)</f>
+        <f t="shared" si="15"/>
         <v>7578.1698572618807</v>
       </c>
       <c r="AE46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AE41*AE42)+AE43+2*AE44)</f>
+        <f t="shared" si="15"/>
         <v>8638.3249754910394</v>
       </c>
       <c r="AF46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AF41*AF42)+AF43+2*AF44)</f>
+        <f t="shared" si="15"/>
         <v>10216.329730080697</v>
       </c>
       <c r="AG46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AG41*AG42)+AG43+2*AG44)</f>
+        <f t="shared" si="15"/>
         <v>11851.389295709534</v>
       </c>
       <c r="AH46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AH41*AH42)+AH43+2*AH44)</f>
+        <f t="shared" si="15"/>
         <v>7798.0427317157837</v>
       </c>
       <c r="AI46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AI41*AI42)+AI43+2*AI44)</f>
+        <f t="shared" si="15"/>
         <v>9823.2831380304742</v>
       </c>
       <c r="AJ46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AJ41*AJ42)+AJ43+2*AJ44)</f>
+        <f t="shared" si="15"/>
         <v>12085.037771363232</v>
       </c>
       <c r="AK46" s="31">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AK41*AK42)+AK43+2*AK44)</f>
+        <f t="shared" si="15"/>
         <v>13929.707718142745</v>
       </c>
       <c r="AL46" s="37">
-        <f>((2*PI()^2)/($G$15^2))*(SQRT(AL41*AL42)+AL43+2*AL44)</f>
+        <f t="shared" si="15"/>
         <v>11250.659189393227</v>
       </c>
     </row>
@@ -3220,95 +3412,95 @@
         <v>49</v>
       </c>
       <c r="P47" s="49">
-        <f>ABS($F$9/P46)</f>
+        <f t="shared" ref="P47:AL47" si="16">ABS($F$9/P46)</f>
         <v>111.33886125761367</v>
       </c>
       <c r="Q47" s="49">
-        <f>ABS($F$9/Q46)</f>
+        <f t="shared" si="16"/>
         <v>46.019787173663836</v>
       </c>
       <c r="R47" s="49">
-        <f>ABS($F$9/R46)</f>
+        <f t="shared" si="16"/>
         <v>27.104794152367663</v>
       </c>
       <c r="S47" s="49">
-        <f>ABS($F$9/S46)</f>
+        <f t="shared" si="16"/>
         <v>27.923298274948177</v>
       </c>
       <c r="T47" s="49">
-        <f>ABS($F$9/T46)</f>
+        <f t="shared" si="16"/>
         <v>18.021819765164462</v>
       </c>
       <c r="U47" s="49">
-        <f>ABS($F$9/U46)</f>
+        <f t="shared" si="16"/>
         <v>11.148558771711397</v>
       </c>
       <c r="V47" s="49">
-        <f>ABS($F$9/V46)</f>
+        <f t="shared" si="16"/>
         <v>11.021307529743982</v>
       </c>
       <c r="W47" s="49">
-        <f>ABS($F$9/W46)</f>
+        <f t="shared" si="16"/>
         <v>8.6484377846817253</v>
       </c>
       <c r="X47" s="49">
-        <f>ABS($F$9/X46)</f>
+        <f t="shared" si="16"/>
         <v>6.6282139291785551</v>
       </c>
       <c r="Y47" s="49">
-        <f>ABS($F$9/Y46)</f>
+        <f t="shared" si="16"/>
         <v>4.5923321100485195</v>
       </c>
       <c r="Z47" s="49">
-        <f>ABS($F$9/Z46)</f>
+        <f t="shared" si="16"/>
         <v>3.3560372500232147</v>
       </c>
       <c r="AA47" s="49">
-        <f>ABS($F$9/AA46)</f>
+        <f t="shared" si="16"/>
         <v>2.8312646651388209</v>
       </c>
       <c r="AB47" s="49">
-        <f>ABS($F$9/AB46)</f>
+        <f t="shared" si="16"/>
         <v>2.3620004134244903</v>
       </c>
       <c r="AC47" s="49">
-        <f>ABS($F$9/AC46)</f>
+        <f t="shared" si="16"/>
         <v>1.815382933455995</v>
       </c>
       <c r="AD47" s="49">
-        <f>ABS($F$9/AD46)</f>
+        <f t="shared" si="16"/>
         <v>1.4357728180428799</v>
       </c>
       <c r="AE47" s="49">
-        <f>ABS($F$9/AE46)</f>
+        <f t="shared" si="16"/>
         <v>1.2595648256391283</v>
       </c>
       <c r="AF47" s="49">
-        <f>ABS($F$9/AF46)</f>
+        <f t="shared" si="16"/>
         <v>1.0650136182989618</v>
       </c>
       <c r="AG47" s="49">
-        <f>ABS($F$9/AG46)</f>
+        <f t="shared" si="16"/>
         <v>0.91808057435996071</v>
       </c>
       <c r="AH47" s="49">
-        <f>ABS($F$9/AH46)</f>
+        <f t="shared" si="16"/>
         <v>1.395289903621044</v>
       </c>
       <c r="AI47" s="49">
-        <f>ABS($F$9/AI46)</f>
+        <f t="shared" si="16"/>
         <v>1.1076266599142328</v>
       </c>
       <c r="AJ47" s="49">
-        <f>ABS($F$9/AJ46)</f>
+        <f t="shared" si="16"/>
         <v>0.90033068141094763</v>
       </c>
       <c r="AK47" s="49">
-        <f>ABS($F$9/AK46)</f>
+        <f t="shared" si="16"/>
         <v>0.78110255518119409</v>
       </c>
       <c r="AL47" s="50">
-        <f>ABS($F$9/AL46)</f>
+        <f t="shared" si="16"/>
         <v>0.96710158119680001</v>
       </c>
     </row>
@@ -3505,35 +3697,35 @@
         <v>0.11943999999999999</v>
       </c>
       <c r="R64">
-        <f t="shared" ref="R64:Z64" si="15">$Z$64*R63</f>
+        <f t="shared" ref="R64:Y64" si="17">$Z$64*R63</f>
         <v>0.23887999999999998</v>
       </c>
       <c r="S64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.35831999999999997</v>
       </c>
       <c r="T64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.47775999999999996</v>
       </c>
       <c r="U64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.59719999999999995</v>
       </c>
       <c r="V64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.71663999999999994</v>
       </c>
       <c r="W64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.83607999999999993</v>
       </c>
       <c r="X64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.95551999999999992</v>
       </c>
       <c r="Y64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.0749599999999999</v>
       </c>
       <c r="Z64">
@@ -3590,27 +3782,27 @@
         <v>9.8301000000000013E-2</v>
       </c>
       <c r="R66">
-        <f t="shared" ref="R66:Y66" si="16">$AC$66*R63+$P$66</f>
+        <f t="shared" ref="R66:Y66" si="18">$AC$66*R63+$P$66</f>
         <v>9.645200000000001E-2</v>
       </c>
       <c r="S66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.4603000000000007E-2</v>
       </c>
       <c r="T66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.2754000000000003E-2</v>
       </c>
       <c r="U66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.0905000000000014E-2</v>
       </c>
       <c r="V66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.905600000000001E-2</v>
       </c>
       <c r="W66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7207000000000007E-2</v>
       </c>
       <c r="X66">
@@ -3618,7 +3810,7 @@
         <v>8.5358000000000003E-2</v>
       </c>
       <c r="Y66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.3509E-2</v>
       </c>
       <c r="Z66">
@@ -3638,39 +3830,39 @@
         <v>0.55082500000000012</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67:Y67" si="17">$I$15*Q64+$J$9</f>
+        <f t="shared" ref="Q67:Y67" si="19">$I$15*Q64+$J$9</f>
         <v>0.54065550000000007</v>
       </c>
       <c r="R67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.53048600000000012</v>
       </c>
       <c r="S67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.52031650000000007</v>
       </c>
       <c r="T67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.51014700000000002</v>
       </c>
       <c r="U67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.49997750000000007</v>
       </c>
       <c r="V67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.48980800000000002</v>
       </c>
       <c r="W67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.47963850000000002</v>
       </c>
       <c r="X67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.46946900000000003</v>
       </c>
       <c r="Y67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.45929949999999997</v>
       </c>
       <c r="Z67">
@@ -3687,23 +3879,23 @@
         <v>-10880.530703056706</v>
       </c>
       <c r="Q68">
-        <f t="shared" ref="Q68:U68" si="18">Q65/(Q66*Q67)</f>
+        <f t="shared" ref="Q68:U68" si="20">Q65/(Q66*Q67)</f>
         <v>-9126.2332336724976</v>
       </c>
       <c r="R68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>-7467.7751798585723</v>
       </c>
       <c r="S68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>-5920.5262227184921</v>
       </c>
       <c r="T68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>-4501.8745444045271</v>
       </c>
       <c r="U68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>-3231.5143924356516</v>
       </c>
       <c r="V68">
@@ -3711,19 +3903,19 @@
         <v>-2131.7799300139641</v>
       </c>
       <c r="W68">
-        <f t="shared" ref="W68" si="19">W65/(W66*W67)</f>
+        <f t="shared" ref="W68" si="21">W65/(W66*W67)</f>
         <v>-1228.033827804049</v>
       </c>
       <c r="X68">
-        <f t="shared" ref="X68" si="20">X65/(X66*X67)</f>
+        <f t="shared" ref="X68" si="22">X65/(X66*X67)</f>
         <v>-549.1207986867305</v>
       </c>
       <c r="Y68">
-        <f t="shared" ref="Y68" si="21">Y65/(Y66*Y67)</f>
+        <f t="shared" ref="Y68" si="23">Y65/(Y66*Y67)</f>
         <v>-127.8984281717108</v>
       </c>
       <c r="Z68">
-        <f t="shared" ref="Z68" si="22">Z65/(Z66*Z67)</f>
+        <f t="shared" ref="Z68" si="24">Z65/(Z66*Z67)</f>
         <v>-1.8603144258741475</v>
       </c>
     </row>
@@ -3783,39 +3975,39 @@
         <v>11250.659189393227</v>
       </c>
       <c r="R71" s="1">
-        <f t="shared" ref="R71:Z71" si="23">$P$71</f>
+        <f t="shared" ref="R71:Z71" si="25">$P$71</f>
         <v>11250.659189393227</v>
       </c>
       <c r="S71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="T71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="U71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="V71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="W71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="X71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="Y71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
       <c r="Z71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>11250.659189393227</v>
       </c>
     </row>
@@ -3834,43 +4026,43 @@
         <v>0.96710161777138648</v>
       </c>
       <c r="Q72" s="46">
-        <f t="shared" ref="Q72:Z72" si="24">ABS(Q68/Q71)</f>
+        <f t="shared" ref="Q72:Z72" si="26">ABS(Q68/Q71)</f>
         <v>0.81117320150239969</v>
       </c>
       <c r="R72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.66376334525349046</v>
       </c>
       <c r="S72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.52623816285362024</v>
       </c>
       <c r="T72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.40014317993462595</v>
       </c>
       <c r="U72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.28722889370626598</v>
       </c>
       <c r="V72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.18948044680117412</v>
       </c>
       <c r="W72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.10915216674253196</v>
       </c>
       <c r="X72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>4.880787778234582E-2</v>
       </c>
       <c r="Y72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.13680830623942E-2</v>
       </c>
       <c r="Z72" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.6535159358733347E-4</v>
       </c>
     </row>
@@ -3886,43 +4078,43 @@
         <v>1.3952899563891836</v>
       </c>
       <c r="Q73" s="1">
-        <f t="shared" ref="Q73:Z73" si="25">ABS(Q68/$AH$46)</f>
+        <f t="shared" ref="Q73:Z73" si="27">ABS(Q68/$AH$46)</f>
         <v>1.1703235731903299</v>
       </c>
       <c r="R73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.95764737855129145</v>
       </c>
       <c r="S73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.75923233898665921</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.57730826814974268</v>
       </c>
       <c r="U73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.41440070330630641</v>
       </c>
       <c r="V73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.27337371740009869</v>
       </c>
       <c r="W73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.15747975101616912</v>
       </c>
       <c r="X73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>7.0417772456333905E-2</v>
       </c>
       <c r="Y73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>1.6401350001780463E-2</v>
       </c>
       <c r="Z73" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>2.3856171219836689E-4</v>
       </c>
     </row>
@@ -4755,7 +4947,7 @@
         <v>6</v>
       </c>
       <c r="Z20">
-        <f>SUM(V20:Y20)</f>
+        <f t="shared" ref="Z20:Z25" si="1">SUM(V20:Y20)</f>
         <v>14</v>
       </c>
     </row>
@@ -4830,7 +5022,7 @@
         <v>4</v>
       </c>
       <c r="Z21">
-        <f>SUM(V21:Y21)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -4905,7 +5097,7 @@
         <v>4</v>
       </c>
       <c r="Z22">
-        <f>SUM(V22:Y22)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -4980,7 +5172,7 @@
         <v>3</v>
       </c>
       <c r="Z23">
-        <f>SUM(V23:Y23)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -5055,7 +5247,7 @@
         <v>2</v>
       </c>
       <c r="Z24">
-        <f>SUM(V24:Y24)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -5130,7 +5322,7 @@
         <v>2</v>
       </c>
       <c r="Z25">
-        <f>SUM(V25:Y25)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -5396,7 +5588,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43:G61" si="1">((2*PI()^2)/F43^2)*(SQRT(B43*C43)+D43+2*E43)</f>
+        <f t="shared" ref="G43:G61" si="2">((2*PI()^2)/F43^2)*(SQRT(B43*C43)+D43+2*E43)</f>
         <v>8851.7803200235103</v>
       </c>
     </row>
@@ -5421,7 +5613,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6501.0937022083972</v>
       </c>
     </row>
@@ -5446,7 +5638,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5689.9576884954422</v>
       </c>
     </row>
@@ -5471,7 +5663,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4264.5137751290276</v>
       </c>
     </row>
@@ -5496,7 +5688,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3041.6378373950474</v>
       </c>
     </row>
@@ -5521,7 +5713,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1924.1948154928991</v>
       </c>
     </row>
@@ -5546,7 +5738,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1575.6314136504807</v>
       </c>
     </row>
@@ -5571,7 +5763,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1010.8668227129787</v>
       </c>
     </row>
@@ -5596,7 +5788,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>570.97256977281052</v>
       </c>
     </row>
@@ -5621,7 +5813,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>231.9521406474866</v>
       </c>
     </row>
@@ -5646,7 +5838,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>157.13153843933841</v>
       </c>
     </row>
@@ -5671,7 +5863,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60.324126929341098</v>
       </c>
     </row>
@@ -5696,7 +5888,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.2702019611697128</v>
       </c>
     </row>
@@ -5721,7 +5913,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7823.8098846423736</v>
       </c>
       <c r="K56" s="57"/>
@@ -5755,7 +5947,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5330.3828954855308</v>
       </c>
       <c r="M57" s="57"/>
@@ -5787,7 +5979,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3515.0063564270372</v>
       </c>
       <c r="N58" s="57"/>
@@ -5818,7 +6010,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2015.188464951229</v>
       </c>
       <c r="P59" s="57"/>
@@ -5847,7 +6039,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1056.9553640328454</v>
       </c>
       <c r="Q60" s="57"/>
@@ -5875,7 +6067,7 @@
         <v>1.1943999999999999</v>
       </c>
       <c r="G61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>465.4641526401806</v>
       </c>
       <c r="R61" s="57"/>
@@ -5890,4 +6082,1673 @@
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042D8D2E-B174-48C2-A489-3514EDBEF371}">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="9.06640625" customWidth="1"/>
+    <col min="10" max="10" width="20.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1">
+        <v>0.44912999999999997</v>
+      </c>
+      <c r="C1">
+        <v>0.15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2">
+        <v>0.55082500000000001</v>
+      </c>
+      <c r="C2">
+        <f>B2-(2*0.15)</f>
+        <v>0.25082500000000002</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2">
+        <v>25.609400000000001</v>
+      </c>
+      <c r="L2">
+        <v>43.566800000000001</v>
+      </c>
+      <c r="M2">
+        <v>151.38399999999999</v>
+      </c>
+      <c r="N2">
+        <v>156.893</v>
+      </c>
+      <c r="O2">
+        <v>106.78700000000001</v>
+      </c>
+      <c r="P2">
+        <v>183.48400000000001</v>
+      </c>
+      <c r="Q2">
+        <v>276.26600000000002</v>
+      </c>
+      <c r="R2">
+        <v>323.94799999999998</v>
+      </c>
+      <c r="S2">
+        <v>28.894600000000001</v>
+      </c>
+      <c r="T2">
+        <v>19.833600000000001</v>
+      </c>
+      <c r="U2">
+        <v>25.228000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <v>1.1943999999999999</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3">
+        <v>11.2498</v>
+      </c>
+      <c r="L3">
+        <v>14.637499999999999</v>
+      </c>
+      <c r="M3">
+        <v>30.5501</v>
+      </c>
+      <c r="N3">
+        <v>32.283799999999999</v>
+      </c>
+      <c r="O3">
+        <v>14.831300000000001</v>
+      </c>
+      <c r="P3">
+        <v>51.142600000000002</v>
+      </c>
+      <c r="Q3">
+        <v>53.475099999999998</v>
+      </c>
+      <c r="R3">
+        <v>65.863900000000001</v>
+      </c>
+      <c r="S3">
+        <v>14.1114</v>
+      </c>
+      <c r="T3">
+        <v>6.6787400000000003</v>
+      </c>
+      <c r="U3">
+        <v>11.811500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4">
+        <v>36.974299999999999</v>
+      </c>
+      <c r="L4">
+        <v>48.302199999999999</v>
+      </c>
+      <c r="M4">
+        <v>74.671599999999998</v>
+      </c>
+      <c r="N4">
+        <v>143.63399999999999</v>
+      </c>
+      <c r="O4">
+        <v>84.733800000000002</v>
+      </c>
+      <c r="P4">
+        <v>170.22499999999999</v>
+      </c>
+      <c r="Q4">
+        <v>177.636</v>
+      </c>
+      <c r="R4">
+        <v>203.09299999999999</v>
+      </c>
+      <c r="S4">
+        <v>42.820300000000003</v>
+      </c>
+      <c r="T4">
+        <v>33.759300000000003</v>
+      </c>
+      <c r="U4">
+        <v>18.099399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5">
+        <v>3.65299</v>
+      </c>
+      <c r="L5">
+        <v>17.095199999999998</v>
+      </c>
+      <c r="M5">
+        <v>36.375599999999999</v>
+      </c>
+      <c r="N5">
+        <v>39.690399999999997</v>
+      </c>
+      <c r="O5">
+        <v>19.3184</v>
+      </c>
+      <c r="P5">
+        <v>60.393300000000004</v>
+      </c>
+      <c r="Q5">
+        <v>64.852999999999994</v>
+      </c>
+      <c r="R5">
+        <v>70.093000000000004</v>
+      </c>
+      <c r="S5">
+        <v>14.7529</v>
+      </c>
+      <c r="T5">
+        <v>7.1085399999999996</v>
+      </c>
+      <c r="U5">
+        <v>12.241300000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <f>B2/B3</f>
+        <v>0.46117297387809786</v>
+      </c>
+      <c r="C7">
+        <f>C2/B3</f>
+        <v>0.21000083724045548</v>
+      </c>
+      <c r="J7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K7">
+        <f>K2*$B$4^4*$B$7^4</f>
+        <v>18.534239890173581</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:S7" si="0">L2*$B$4^4*$B$7^4</f>
+        <v>31.530513110311617</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>109.56083982967336</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>113.54785739177815</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>77.284742131872122</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>132.7925086885522</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>199.94144015473591</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>234.45023873819574</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>20.911831121799398</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:U7" si="1">T2*$B$4^4*$B$7^4</f>
+        <v>14.354131697179422</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="1"/>
+        <v>18.258210030274004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8">
+        <f>B1/B3</f>
+        <v>0.37602980576021433</v>
+      </c>
+      <c r="C8">
+        <f>C1/B3</f>
+        <v>0.12558606831882116</v>
+      </c>
+      <c r="J8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K8">
+        <f>K2*$B$4^4*$B$8^4</f>
+        <v>8.1923494220633657</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:S8" si="2">L2*$B$4^4*$B$8^4</f>
+        <v>13.936853218003945</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>48.427164436091452</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>50.189472532577398</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>34.160754165809458</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>58.695832052210307</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>88.376440113230217</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>103.62973012169684</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>9.2432723769690863</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:U8" si="3">T2*$B$4^4*$B$8^4</f>
+        <v>6.344693022774293</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="3"/>
+        <v>8.0703410161821285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="J9" t="s">
+        <v>155</v>
+      </c>
+      <c r="K9">
+        <f>2*(K3+2*K5)*$B$4^2*$B$5^2*$B$7^4</f>
+        <v>6.7146687909378011</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:S9" si="4">2*(L3+2*L5)*$B$4^2*$B$5^2*$B$7^4</f>
+        <v>17.669059250380847</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>37.381021717939269</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>40.407398916809385</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>19.348180587436449</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>62.214988186479019</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>66.286645738398306</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>74.562041202571649</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>15.783494500802028</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ref="T9:U9" si="5">2*(T3+2*T5)*$B$4^2*$B$5^2*$B$7^4</f>
+        <v>7.5614450276438898</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="5"/>
+        <v>13.133528235685898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10">
+        <f>(1740.1)+77.8704</f>
+        <v>1817.9703999999999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10">
+        <f>B10/B1</f>
+        <v>4047.7598913454904</v>
+      </c>
+      <c r="J10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10">
+        <f>2*(K3+2*K5)*$B$4^2*$B$5^2*$B$8^4</f>
+        <v>2.9679616382838909</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:S10" si="6">2*(L3+2*L5)*$B$4^2*$B$5^2*$B$8^4</f>
+        <v>7.8099295248144784</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="6"/>
+        <v>16.522846012663209</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="6"/>
+        <v>17.860539904779824</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>8.552120669243056</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>27.499747792916214</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="6"/>
+        <v>29.299467748520691</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="6"/>
+        <v>32.957288713933444</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>6.9764879929249064</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ref="T10:U10" si="7">2*(T3+2*T5)*$B$4^2*$B$5^2*$B$8^4</f>
+        <v>3.3422465754867376</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="7"/>
+        <v>5.8051721078844096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="1">
+        <f>1015.8</f>
+        <v>1015.8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="49">
+        <f>B11/B3</f>
+        <v>850.46885465505693</v>
+      </c>
+      <c r="J11" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11">
+        <f>K4*$B$5^4</f>
+        <v>36.974299999999999</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:R11" si="8">L4*$B$5^4</f>
+        <v>48.302199999999999</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="8"/>
+        <v>74.671599999999998</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="8"/>
+        <v>143.63399999999999</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="8"/>
+        <v>84.733800000000002</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="8"/>
+        <v>170.22499999999999</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="8"/>
+        <v>177.636</v>
+      </c>
+      <c r="R11">
+        <f>R4*$B$5^4</f>
+        <v>203.09299999999999</v>
+      </c>
+      <c r="S11">
+        <f>S4*$B$5^4</f>
+        <v>42.820300000000003</v>
+      </c>
+      <c r="T11">
+        <f>T4*$B$5^4</f>
+        <v>33.759300000000003</v>
+      </c>
+      <c r="U11">
+        <f>U4*$B$5^4</f>
+        <v>18.099399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12">
+        <f>B11/B10</f>
+        <v>0.55875497202814739</v>
+      </c>
+      <c r="J12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12">
+        <f>(PI()^2/$B$7^2)*(K7+K9+K11)</f>
+        <v>2887.5163452860052</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12:M12" si="9">(PI()^2/$B$7^2)*(L7+L9+L11)</f>
+        <v>4524.6455037173137</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="9"/>
+        <v>10284.144873235964</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12" si="10">(PI()^2/$B$7^2)*(N7+N9+N11)</f>
+        <v>13809.8606610977</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12" si="11">(PI()^2/$B$7^2)*(O7+O9+O11)</f>
+        <v>8416.4636868354482</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ref="P12" si="12">(PI()^2/$B$7^2)*(P7+P9+P11)</f>
+        <v>16948.897797300731</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12" si="13">(PI()^2/$B$7^2)*(Q7+Q9+Q11)</f>
+        <v>20597.857781174203</v>
+      </c>
+      <c r="R12">
+        <f>(PI()^2/$B$7^2)*(R7+R9+R11)</f>
+        <v>23764.643413272133</v>
+      </c>
+      <c r="S12">
+        <f t="shared" ref="S12:U12" si="14">(PI()^2/$B$7^2)*(S7+S9+S11)</f>
+        <v>3689.9843893875409</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="14"/>
+        <v>2583.6359129051471</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="14"/>
+        <v>2296.6747250556032</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="J13" t="s">
+        <v>158</v>
+      </c>
+      <c r="K13">
+        <f>(PI()^2/$B$7^2)*(K8+K10+K11)</f>
+        <v>2233.7240260791818</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13:R13" si="15">(PI()^2/$B$7^2)*(L8+L10+L11)</f>
+        <v>3250.6774711209373</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="15"/>
+        <v>6479.2493166351042</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="15"/>
+        <v>9823.3610722512403</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="15"/>
+        <v>5914.261969750798</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="15"/>
+        <v>11899.396242406912</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="15"/>
+        <v>13704.178536958887</v>
+      </c>
+      <c r="R13">
+        <f>(PI()^2/$B$7^2)*(R8+R10+R11)</f>
+        <v>15763.115200015136</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ref="S13:T13" si="16">(PI()^2/$B$7^2)*(S8+S10+S11)</f>
+        <v>2739.79987464858</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ref="T13:U13" si="17">(PI()^2/$B$7^2)*(T8+T10+T11)</f>
+        <v>2016.1565055913488</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="17"/>
+        <v>1483.8206875189555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="J15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15">
+        <f>($B$4^2)*$B$7^2+$B$12*$B$5^2</f>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="L15">
+        <f>($B$4^2)*$B$7^2+$B$12*$B$5^2</f>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="M15">
+        <f>($B$4^2)*$B$7^2+$B$12*$B$5^2</f>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="N15">
+        <f>($B$4^2)*$B$7^2+$B$12*$B$5^2</f>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="O15">
+        <f>($B$4^2)*$B$7^2+$B$12*$B$5^2</f>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="P15">
+        <f t="shared" ref="P15:U15" si="18">($B$4^2)*$B$7^2+$B$12*$B$5^2</f>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="18"/>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="18"/>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="18"/>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="18"/>
+        <v>1.4094770193704225</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="18"/>
+        <v>1.4094770193704225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16">
+        <v>-600.22580000000005</v>
+      </c>
+      <c r="C16" t="s">
+        <v>194</v>
+      </c>
+      <c r="J16" t="s">
+        <v>139</v>
+      </c>
+      <c r="K16">
+        <f>($B$4^2)*$B$8^2+$B$12*$B$5^2</f>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="L16">
+        <f>($B$4^2)*$B$8^2+$B$12*$B$5^2</f>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="M16">
+        <f>($B$4^2)*$B$8^2+$B$12*$B$5^2</f>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="N16">
+        <f>($B$4^2)*$B$8^2+$B$12*$B$5^2</f>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="O16">
+        <f>($B$4^2)*$B$8^2+$B$12*$B$5^2</f>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ref="P16:U16" si="19">($B$4^2)*$B$8^2+$B$12*$B$5^2</f>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="19"/>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="19"/>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="19"/>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="19"/>
+        <v>1.1243486313084055</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="19"/>
+        <v>1.1243486313084055</v>
+      </c>
+    </row>
+    <row r="19" spans="10:21" x14ac:dyDescent="0.45">
+      <c r="J19" t="s">
+        <v>140</v>
+      </c>
+      <c r="K19">
+        <f>K12/K15</f>
+        <v>2048.6437917063631</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ref="L19:T19" si="20">L12/L15</f>
+        <v>3210.1591168463019</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="20"/>
+        <v>7296.4260728632735</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="20"/>
+        <v>9797.8615268705926</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="20"/>
+        <v>5971.3380006684101</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="20"/>
+        <v>12024.955046710427</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="20"/>
+        <v>14613.830164024059</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="20"/>
+        <v>16860.610770289248</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="20"/>
+        <v>2617.9812360727692</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="20"/>
+        <v>1833.0457874788135</v>
+      </c>
+      <c r="U19">
+        <f t="shared" ref="U19" si="21">U12/U15</f>
+        <v>1629.4516998095289</v>
+      </c>
+    </row>
+    <row r="20" spans="10:21" x14ac:dyDescent="0.45">
+      <c r="J20" t="s">
+        <v>141</v>
+      </c>
+      <c r="K20">
+        <f>K19*$B$12</f>
+        <v>1144.6899045305267</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ref="L20:O20" si="22">L19*$B$12</f>
+        <v>1793.6923675393577</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="22"/>
+        <v>4076.9143462481638</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="22"/>
+        <v>5474.6038433822396</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="22"/>
+        <v>3336.514797534091</v>
+      </c>
+      <c r="P20">
+        <f t="shared" ref="P20" si="23">P19*$B$12</f>
+        <v>6719.0034207644148</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ref="Q20" si="24">Q19*$B$12</f>
+        <v>8165.5502645233591</v>
+      </c>
+      <c r="R20">
+        <f t="shared" ref="R20:T20" si="25">R19*$B$12</f>
+        <v>9420.95009933045</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="25"/>
+        <v>1462.8100323320548</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="25"/>
+        <v>1024.2234477090378</v>
+      </c>
+      <c r="U20">
+        <f t="shared" ref="U20" si="26">U19*$B$12</f>
+        <v>910.46423894829059</v>
+      </c>
+    </row>
+    <row r="22" spans="10:21" x14ac:dyDescent="0.45">
+      <c r="J22" t="s">
+        <v>142</v>
+      </c>
+      <c r="K22">
+        <f>K13/K16</f>
+        <v>1986.682745795488</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ref="L22:N22" si="27">L13/L16</f>
+        <v>2891.1650537948549</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="27"/>
+        <v>5762.6692790964635</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="27"/>
+        <v>8736.9351451246821</v>
+      </c>
+      <c r="O22">
+        <f>O13/O16</f>
+        <v>5260.167358293812</v>
+      </c>
+      <c r="P22">
+        <f t="shared" ref="P22:T22" si="28">P13/P16</f>
+        <v>10583.36881555997</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="28"/>
+        <v>12188.549134454252</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="28"/>
+        <v>14019.775326867775</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="28"/>
+        <v>2436.78855326241</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="28"/>
+        <v>1793.177355714967</v>
+      </c>
+      <c r="U22">
+        <f t="shared" ref="U22" si="29">U13/U16</f>
+        <v>1319.7158303045489</v>
+      </c>
+    </row>
+    <row r="23" spans="10:21" x14ac:dyDescent="0.45">
+      <c r="J23" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23">
+        <f>$B$12*K22</f>
+        <v>1110.068862055761</v>
+      </c>
+      <c r="L23">
+        <f>$B$12*L22</f>
+        <v>1615.4528487619014</v>
+      </c>
+      <c r="M23">
+        <f>$B$12*M22</f>
+        <v>3219.9201118490087</v>
+      </c>
+      <c r="N23">
+        <f>$B$12*N22</f>
+        <v>4881.8059526258794</v>
+      </c>
+      <c r="O23">
+        <f>$B$12*O22</f>
+        <v>2939.1446651468327</v>
+      </c>
+      <c r="P23">
+        <f t="shared" ref="P23:T23" si="30">$B$12*P22</f>
+        <v>5913.5099465017784</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="30"/>
+        <v>6810.4124306856856</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="30"/>
+        <v>7833.6191706049149</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="30"/>
+        <v>1361.5677199166475</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="30"/>
+        <v>1001.9467632340237</v>
+      </c>
+      <c r="U23">
+        <f t="shared" ref="U23" si="31">$B$12*U22</f>
+        <v>737.39778184692159</v>
+      </c>
+    </row>
+    <row r="25" spans="10:21" x14ac:dyDescent="0.45">
+      <c r="J25" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25">
+        <f>8*2*0.125</f>
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <f>9*2*0.125</f>
+        <v>2.25</v>
+      </c>
+      <c r="M25">
+        <f>12*2*0.125</f>
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>3.25</v>
+      </c>
+      <c r="P25">
+        <v>3.5</v>
+      </c>
+      <c r="Q25">
+        <f>2*15*0.125</f>
+        <v>3.75</v>
+      </c>
+      <c r="S25">
+        <v>2</v>
+      </c>
+      <c r="T25">
+        <v>1.75</v>
+      </c>
+      <c r="U25">
+        <v>1.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992F5B32-D0D4-4B39-B726-B052BEA90962}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1">
+        <v>45</v>
+      </c>
+      <c r="D1">
+        <v>90</v>
+      </c>
+      <c r="E1">
+        <v>-45</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>45</v>
+      </c>
+      <c r="H1">
+        <v>90</v>
+      </c>
+      <c r="I1">
+        <v>-45</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>90</v>
+      </c>
+      <c r="E2">
+        <v>-45</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <v>90</v>
+      </c>
+      <c r="J2">
+        <v>-45</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3">
+        <v>-45</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>90</v>
+      </c>
+      <c r="H3">
+        <v>-45</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
+      <c r="L3">
+        <v>90</v>
+      </c>
+      <c r="M3">
+        <v>-45</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>-45</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>90</v>
+      </c>
+      <c r="I4">
+        <v>-45</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>45</v>
+      </c>
+      <c r="M4">
+        <v>90</v>
+      </c>
+      <c r="N4">
+        <v>-45</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>-45</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>45</v>
+      </c>
+      <c r="L5">
+        <v>-45</v>
+      </c>
+      <c r="M5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>-45</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>45</v>
+      </c>
+      <c r="I6">
+        <v>90</v>
+      </c>
+      <c r="J6">
+        <v>-45</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>45</v>
+      </c>
+      <c r="N6">
+        <v>90</v>
+      </c>
+      <c r="O6">
+        <v>-45</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>-45</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>45</v>
+      </c>
+      <c r="J7">
+        <v>90</v>
+      </c>
+      <c r="K7">
+        <v>-45</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>45</v>
+      </c>
+      <c r="O7">
+        <v>90</v>
+      </c>
+      <c r="P7">
+        <v>-45</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>-45</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>45</v>
+      </c>
+      <c r="J8">
+        <v>90</v>
+      </c>
+      <c r="K8">
+        <v>-45</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>45</v>
+      </c>
+      <c r="O8">
+        <v>90</v>
+      </c>
+      <c r="P8">
+        <v>-45</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CE0D58-5C85-44D1-BFCA-F77F378651F8}">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1">
+        <v>0.44912999999999997</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2">
+        <v>0.55082500000000001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" s="1">
+        <v>67650000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <v>1.1943999999999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43902100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4">
+        <v>1.0015000000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>174</v>
+      </c>
+      <c r="M4" s="1">
+        <v>16115600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5">
+        <v>0.81659999999999999</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.32194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.20891999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8">
+        <f>0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="E8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <f>B3/B1</f>
+        <v>2.6593636586289047</v>
+      </c>
+      <c r="E10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11">
+        <f>B3/B2</f>
+        <v>2.1683837879544319</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="49">
+        <f>B1/SQRT(B6*B7)</f>
+        <v>10.042852107344805</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="49">
+        <f>B2/SQRT(B6*B7)</f>
+        <v>12.316821437063217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>184</v>
+      </c>
+      <c r="G18" s="1">
+        <v>135000000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="1">
+        <v>8500000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20">
+        <v>0.6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>182</v>
+      </c>
+      <c r="J20" s="1">
+        <f>G20*G18+G19*G21</f>
+        <v>84400000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8500000000</v>
+      </c>
+      <c r="F21" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21">
+        <f>1-G20</f>
+        <v>0.4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>183</v>
+      </c>
+      <c r="J21" s="1">
+        <f>1/((G20/G18)+(G21/G19))</f>
+        <v>19416243654.82233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="1">
+        <f>B18*B21*(B6/B1)^2</f>
+        <v>3539599.1457210188</v>
+      </c>
+      <c r="C22" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1650000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="1">
+        <f>B19*B21*(B6/B2)^2</f>
+        <v>2913566.7936804499</v>
+      </c>
+      <c r="C23" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1350000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>188</v>
+      </c>
+      <c r="G24" s="1">
+        <v>79000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F25" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" s="1">
+        <v>230000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F26" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="1">
+        <v>50000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
composite design finalised and ribs check (minor change but no effect on design)
</commit_message>
<xml_diff>
--- a/PreliminaryAirframe/Composite/Composite_vertical_tailplane_sizing.xlsx
+++ b/PreliminaryAirframe/Composite/Composite_vertical_tailplane_sizing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ca90458c880e139/Documents/GitHub/AVD/PreliminaryAirframe/Composite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1682" documentId="8_{F426B969-63F3-4CD9-9347-CB9329FBF99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{597C73AA-F51C-4C61-A072-906B7AED6B23}"/>
+  <xr:revisionPtr revIDLastSave="1802" documentId="8_{F426B969-63F3-4CD9-9347-CB9329FBF99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4410B56B-EAE5-48E3-A77F-416DD5644A06}"/>
   <bookViews>
-    <workbookView xWindow="-11550" yWindow="3623" windowWidth="19200" windowHeight="8422" firstSheet="1" activeTab="4" xr2:uid="{E7E02545-2DF6-46D5-87DA-A9BD6A8E819A}"/>
+    <workbookView xWindow="9608" yWindow="3533" windowWidth="19200" windowHeight="8422" firstSheet="2" activeTab="5" xr2:uid="{E7E02545-2DF6-46D5-87DA-A9BD6A8E819A}"/>
   </bookViews>
   <sheets>
     <sheet name="1. 0 ribs" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Panel V2" sheetId="3" r:id="rId3"/>
     <sheet name="Panel Design V2" sheetId="4" r:id="rId4"/>
     <sheet name="D-CELL V2" sheetId="5" r:id="rId5"/>
+    <sheet name="SPAR V2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="238">
   <si>
     <t>Composite Wingbox sizing</t>
   </si>
@@ -633,6 +634,126 @@
   </si>
   <si>
     <t>2.91 Mpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good! </t>
+  </si>
+  <si>
+    <t>Good!</t>
+  </si>
+  <si>
+    <t>Min E</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>t [mm]</t>
+  </si>
+  <si>
+    <t>c max [mm]</t>
+  </si>
+  <si>
+    <t>c min [mm]</t>
+  </si>
+  <si>
+    <t>b max</t>
+  </si>
+  <si>
+    <t>b min [mm]</t>
+  </si>
+  <si>
+    <t>c/t</t>
+  </si>
+  <si>
+    <t>Core (foam)</t>
+  </si>
+  <si>
+    <t>Facesheets</t>
+  </si>
+  <si>
+    <t>E_f</t>
+  </si>
+  <si>
+    <t>E_c</t>
+  </si>
+  <si>
+    <t>E [Pa]</t>
+  </si>
+  <si>
+    <t>sigma_ft</t>
+  </si>
+  <si>
+    <t>sigma_fc</t>
+  </si>
+  <si>
+    <t>tau_c</t>
+  </si>
+  <si>
+    <t>sigma_core</t>
+  </si>
+  <si>
+    <t>sigma_f</t>
+  </si>
+  <si>
+    <t>Al-7075, O</t>
+  </si>
+  <si>
+    <t>P_FS_T</t>
+  </si>
+  <si>
+    <t>P_FS_C</t>
+  </si>
+  <si>
+    <t>d max</t>
+  </si>
+  <si>
+    <t>d min</t>
+  </si>
+  <si>
+    <t>P_IN</t>
+  </si>
+  <si>
+    <t>Shear strength</t>
+  </si>
+  <si>
+    <t>P_CS</t>
+  </si>
+  <si>
+    <t>Compressive strength of foam/ core</t>
+  </si>
+  <si>
+    <t>(EI)_eq</t>
+  </si>
+  <si>
+    <t>P_E</t>
+  </si>
+  <si>
+    <t>Euler buckling load</t>
+  </si>
+  <si>
+    <t>G_c</t>
+  </si>
+  <si>
+    <t>Shear modulus of core</t>
+  </si>
+  <si>
+    <t>P_s</t>
+  </si>
+  <si>
+    <t>shear stiffness of core</t>
+  </si>
+  <si>
+    <t>P_cr</t>
+  </si>
+  <si>
+    <t>Combined Collapse load</t>
+  </si>
+  <si>
+    <t>sigma_fw</t>
+  </si>
+  <si>
+    <t>Face wrinkling</t>
   </si>
 </sst>
 </file>
@@ -795,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -922,6 +1043,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,7 +1360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD7C898-DEA3-436A-978C-3D1D23C43CFE}">
   <dimension ref="A1:AL76"/>
   <sheetViews>
-    <sheetView topLeftCell="M7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
@@ -6089,7 +6211,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6574,7 +6696,7 @@
         <v>36.974299999999999</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:R11" si="8">L4*$B$5^4</f>
+        <f t="shared" ref="L11:Q11" si="8">L4*$B$5^4</f>
         <v>48.302199999999999</v>
       </c>
       <c r="M11">
@@ -6679,7 +6801,7 @@
         <v>2233.7240260791818</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:R13" si="15">(PI()^2/$B$7^2)*(L8+L10+L11)</f>
+        <f t="shared" ref="L13:Q13" si="15">(PI()^2/$B$7^2)*(L8+L10+L11)</f>
         <v>3250.6774711209373</v>
       </c>
       <c r="M13">
@@ -6707,7 +6829,7 @@
         <v>15763.115200015136</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:T13" si="16">(PI()^2/$B$7^2)*(S8+S10+S11)</f>
+        <f t="shared" ref="S13" si="16">(PI()^2/$B$7^2)*(S8+S10+S11)</f>
         <v>2739.79987464858</v>
       </c>
       <c r="T13">
@@ -6769,15 +6891,6 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>193</v>
-      </c>
-      <c r="B16">
-        <v>-600.22580000000005</v>
-      </c>
-      <c r="C16" t="s">
-        <v>194</v>
-      </c>
       <c r="J16" t="s">
         <v>139</v>
       </c>
@@ -7438,8 +7551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CE0D58-5C85-44D1-BFCA-F77F378651F8}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7673,6 +7786,9 @@
       <c r="B21" s="1">
         <v>8500000000</v>
       </c>
+      <c r="D21" t="s">
+        <v>200</v>
+      </c>
       <c r="F21" t="s">
         <v>181</v>
       </c>
@@ -7699,6 +7815,9 @@
       <c r="C22" t="s">
         <v>196</v>
       </c>
+      <c r="D22" t="s">
+        <v>198</v>
+      </c>
       <c r="F22" t="s">
         <v>185</v>
       </c>
@@ -7717,6 +7836,9 @@
       <c r="C23" t="s">
         <v>197</v>
       </c>
+      <c r="D23" t="s">
+        <v>199</v>
+      </c>
       <c r="F23" t="s">
         <v>186</v>
       </c>
@@ -7751,4 +7873,341 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59BF47A-DA40-4E72-9551-B78BF64E221F}">
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1">
+        <v>-600.22580000000005</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1">
+        <v>116.1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2">
+        <v>81.8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H2" s="1">
+        <v>72000000000</v>
+      </c>
+      <c r="K2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L2" s="1">
+        <v>484000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L3">
+        <f>E1-H3</f>
+        <v>115.1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>207</v>
+      </c>
+      <c r="O3">
+        <f>L3/H3</f>
+        <v>115.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1.1943999999999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>218</v>
+      </c>
+      <c r="K4" t="s">
+        <v>204</v>
+      </c>
+      <c r="L4">
+        <f>E2-H3</f>
+        <v>80.8</v>
+      </c>
+      <c r="O4">
+        <f>L4/H3</f>
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <f>L3*10^(-3)</f>
+        <v>0.11509999999999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6">
+        <f>B6+B8</f>
+        <v>0.11609999999999999</v>
+      </c>
+      <c r="G6">
+        <f>B7/B4</f>
+        <v>6.7649028801071667E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7">
+        <f>L4*10^(-3)</f>
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7">
+        <f>B7+B8</f>
+        <v>8.1799999999999998E-2</v>
+      </c>
+      <c r="G7">
+        <f>B8/B7</f>
+        <v>1.2376237623762377E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8">
+        <f>H3*10^(-3)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G8">
+        <f>B8/B6</f>
+        <v>8.6880973066898355E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="1">
+        <f>H2</f>
+        <v>72000000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="1">
+        <f>L2</f>
+        <v>484000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10">
+        <f>ABS(B1)/(B5*B8*(B6+B8))</f>
+        <v>51699035.314384155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="1">
+        <v>214000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="1">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="1">
+        <v>50000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="60">
+        <f>D7*4*B5*B8*B12/B4</f>
+        <v>5862.4246483590096</v>
+      </c>
+      <c r="D18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E18" s="1">
+        <f>B5*B8*B7^2*B9/2</f>
+        <v>23503.103999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="60">
+        <f>4*D7*B5*B8*B13/B4</f>
+        <v>2739.4507702612191</v>
+      </c>
+      <c r="D19" t="s">
+        <v>230</v>
+      </c>
+      <c r="E19" s="1">
+        <f>350000</f>
+        <v>350000</v>
+      </c>
+      <c r="F19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="60">
+        <f>B5*B8*((PI()^2*D7*B9*B15^2)/(3*B4))^(1/3)</f>
+        <v>545.38706311168994</v>
+      </c>
+      <c r="D21" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="1">
+        <f>4*PI()^2*E18/(B4^2)</f>
+        <v>650407.2439571229</v>
+      </c>
+      <c r="F21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="D22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" s="1">
+        <f>B5*B7*E19</f>
+        <v>2828</v>
+      </c>
+      <c r="F22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="60">
+        <f>2*B5*D7*B14</f>
+        <v>818</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="D24" t="s">
+        <v>234</v>
+      </c>
+      <c r="E24" s="1">
+        <f>1/((1/E21)+(1/E22))</f>
+        <v>2815.7569618694288</v>
+      </c>
+      <c r="F24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27" s="1">
+        <f>0.5*(B9*B10*E19)^(1/3)</f>
+        <v>11509381.12912859</v>
+      </c>
+      <c r="F27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>